<commit_message>
[offers][fix] fix base salary for fulltime
</commit_message>
<xml_diff>
--- a/apps/portal/prisma/salaries.xlsx
+++ b/apps/portal/prisma/salaries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stuartlong/Desktop/tech-interview-handbook/apps/portal/prisma/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A645B7-19E9-B54F-909E-60CA88EF3664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70947517-C008-3145-9631-D1512C47BC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2112,10 +2112,10 @@
   <dimension ref="A1:AM660"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D466" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2:E556"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2181,8 +2181,8 @@
         <v>6</v>
       </c>
       <c r="E2" s="9">
-        <f>K2</f>
-        <v>8333</v>
+        <f>K2*12</f>
+        <v>99996</v>
       </c>
       <c r="H2">
         <f>K2*12</f>
@@ -2293,8 +2293,8 @@
         <v>6</v>
       </c>
       <c r="E6" s="9">
-        <f t="shared" ref="E6:E7" si="1">K6</f>
-        <v>5750</v>
+        <f t="shared" ref="E6:E7" si="1">K6*12</f>
+        <v>69000</v>
       </c>
       <c r="G6" s="4">
         <v>1000</v>
@@ -2331,7 +2331,7 @@
       </c>
       <c r="E7" s="9">
         <f t="shared" si="1"/>
-        <v>5400</v>
+        <v>64800</v>
       </c>
       <c r="H7" s="4">
         <v>72300</v>
@@ -2468,8 +2468,8 @@
         <v>291</v>
       </c>
       <c r="E12" s="9">
-        <f t="shared" ref="E12:E13" si="3">K12</f>
-        <v>4167</v>
+        <f t="shared" ref="E12:E13" si="3">K12*12</f>
+        <v>50004</v>
       </c>
       <c r="H12">
         <f>K12*12</f>
@@ -2501,7 +2501,7 @@
       </c>
       <c r="E13" s="9">
         <f t="shared" si="3"/>
-        <v>4600</v>
+        <v>55200</v>
       </c>
       <c r="H13">
         <f>K13*12</f>
@@ -2585,8 +2585,8 @@
         <v>6</v>
       </c>
       <c r="E16" s="9">
-        <f>K16</f>
-        <v>6500</v>
+        <f>K16*12</f>
+        <v>78000</v>
       </c>
       <c r="H16" s="4">
         <v>250000</v>
@@ -2811,8 +2811,8 @@
         <v>6</v>
       </c>
       <c r="E24" s="9">
-        <f t="shared" ref="E24:E25" si="5">K24</f>
-        <v>5600</v>
+        <f t="shared" ref="E24:E25" si="5">K24*12</f>
+        <v>67200</v>
       </c>
       <c r="F24" s="4">
         <v>40000</v>
@@ -2849,7 +2849,7 @@
       </c>
       <c r="E25" s="9">
         <f t="shared" si="5"/>
-        <v>5000</v>
+        <v>60000</v>
       </c>
       <c r="H25" s="4">
         <v>65000</v>
@@ -2987,8 +2987,8 @@
         <v>169</v>
       </c>
       <c r="E30" s="9">
-        <f>K30</f>
-        <v>2900</v>
+        <f>K30*12</f>
+        <v>34800</v>
       </c>
       <c r="H30" s="4">
         <v>37700</v>
@@ -3074,8 +3074,8 @@
         <v>74</v>
       </c>
       <c r="E33" s="9">
-        <f t="shared" ref="E33:E34" si="7">K33</f>
-        <v>5000</v>
+        <f t="shared" ref="E33:E34" si="7">K33*12</f>
+        <v>60000</v>
       </c>
       <c r="F33" s="4">
         <v>0</v>
@@ -3111,7 +3111,7 @@
       </c>
       <c r="E34" s="9">
         <f t="shared" si="7"/>
-        <v>6083</v>
+        <v>72996</v>
       </c>
       <c r="F34" s="4">
         <v>25000</v>
@@ -3369,8 +3369,8 @@
         <v>6</v>
       </c>
       <c r="E43" s="9">
-        <f t="shared" ref="E43:E45" si="9">K43</f>
-        <v>4000</v>
+        <f t="shared" ref="E43:E45" si="9">K43*12</f>
+        <v>48000</v>
       </c>
       <c r="H43">
         <f>K43*12</f>
@@ -3398,7 +3398,7 @@
       </c>
       <c r="E44" s="9">
         <f t="shared" si="9"/>
-        <v>4000</v>
+        <v>48000</v>
       </c>
       <c r="H44">
         <f>K44*12</f>
@@ -3429,7 +3429,7 @@
       </c>
       <c r="E45" s="9">
         <f t="shared" si="9"/>
-        <v>7000</v>
+        <v>84000</v>
       </c>
       <c r="F45" s="4">
         <v>20000</v>
@@ -3635,8 +3635,8 @@
         <v>6</v>
       </c>
       <c r="E52" s="9">
-        <f>K52</f>
-        <v>5100</v>
+        <f>K52*12</f>
+        <v>61200</v>
       </c>
       <c r="H52" s="4">
         <v>61200</v>
@@ -3776,8 +3776,8 @@
         <v>6</v>
       </c>
       <c r="E57" s="9">
-        <f>K57</f>
-        <v>135000</v>
+        <f>K57*12</f>
+        <v>1620000</v>
       </c>
       <c r="F57" s="4">
         <v>0</v>
@@ -3842,8 +3842,8 @@
         <v>6</v>
       </c>
       <c r="E59" s="9">
-        <f>K59</f>
-        <v>9000</v>
+        <f>K59*12</f>
+        <v>108000</v>
       </c>
       <c r="F59" s="4">
         <v>0</v>
@@ -3929,8 +3929,8 @@
         <v>39</v>
       </c>
       <c r="E62" s="9">
-        <f t="shared" ref="E62:E74" si="12">K62</f>
-        <v>14000</v>
+        <f t="shared" ref="E62:E74" si="12">K62*12</f>
+        <v>168000</v>
       </c>
       <c r="F62" s="4">
         <v>200000</v>
@@ -3943,7 +3943,7 @@
       </c>
       <c r="I62" s="4">
         <f>E62*3</f>
-        <v>42000</v>
+        <v>504000</v>
       </c>
       <c r="K62" s="4">
         <v>14000</v>
@@ -3967,7 +3967,7 @@
       </c>
       <c r="E63" s="9">
         <f t="shared" si="12"/>
-        <v>8416</v>
+        <v>100992</v>
       </c>
       <c r="F63" s="4">
         <v>80000</v>
@@ -4001,7 +4001,7 @@
       </c>
       <c r="E64" s="9">
         <f t="shared" si="12"/>
-        <v>7350</v>
+        <v>88200</v>
       </c>
       <c r="F64" s="4">
         <v>22260</v>
@@ -4012,7 +4012,7 @@
       </c>
       <c r="I64" s="4">
         <f t="shared" ref="I64:I71" si="13">E64*1.5</f>
-        <v>11025</v>
+        <v>132300</v>
       </c>
       <c r="K64" s="9">
         <v>7350</v>
@@ -4036,7 +4036,7 @@
       </c>
       <c r="E65" s="9">
         <f t="shared" si="12"/>
-        <v>7200</v>
+        <v>86400</v>
       </c>
       <c r="F65" s="4">
         <v>0</v>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="I65" s="4">
         <f t="shared" si="13"/>
-        <v>10800</v>
+        <v>129600</v>
       </c>
       <c r="J65" s="4" t="s">
         <v>107</v>
@@ -4076,7 +4076,7 @@
       </c>
       <c r="E66" s="9">
         <f t="shared" si="12"/>
-        <v>7200</v>
+        <v>86400</v>
       </c>
       <c r="F66" s="4">
         <v>0</v>
@@ -4089,7 +4089,7 @@
       </c>
       <c r="I66" s="4">
         <f t="shared" si="13"/>
-        <v>10800</v>
+        <v>129600</v>
       </c>
       <c r="K66" s="4">
         <v>7200</v>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="E67" s="9">
         <f t="shared" si="12"/>
-        <v>7000</v>
+        <v>84000</v>
       </c>
       <c r="H67">
         <f>K67*12</f>
@@ -4142,7 +4142,7 @@
       </c>
       <c r="E68" s="9">
         <f t="shared" si="12"/>
-        <v>7000</v>
+        <v>84000</v>
       </c>
       <c r="H68">
         <f>K68*12</f>
@@ -4174,7 +4174,7 @@
       </c>
       <c r="E69" s="9">
         <f t="shared" si="12"/>
-        <v>7000</v>
+        <v>84000</v>
       </c>
       <c r="F69" s="4">
         <v>0</v>
@@ -4187,7 +4187,7 @@
       </c>
       <c r="I69" s="4">
         <f t="shared" si="13"/>
-        <v>10500</v>
+        <v>126000</v>
       </c>
       <c r="J69" s="4" t="s">
         <v>122</v>
@@ -4214,7 +4214,7 @@
       </c>
       <c r="E70" s="9">
         <f t="shared" si="12"/>
-        <v>7000</v>
+        <v>84000</v>
       </c>
       <c r="F70" s="4">
         <v>0</v>
@@ -4227,7 +4227,7 @@
       </c>
       <c r="I70" s="4">
         <f t="shared" si="13"/>
-        <v>10500</v>
+        <v>126000</v>
       </c>
       <c r="K70" s="4">
         <v>7000</v>
@@ -4251,7 +4251,7 @@
       </c>
       <c r="E71" s="9">
         <f t="shared" si="12"/>
-        <v>6800</v>
+        <v>81600</v>
       </c>
       <c r="F71" s="4" t="s">
         <v>132</v>
@@ -4264,7 +4264,7 @@
       </c>
       <c r="I71" s="4">
         <f t="shared" si="13"/>
-        <v>10200</v>
+        <v>122400</v>
       </c>
       <c r="K71" s="9">
         <v>6800</v>
@@ -4288,14 +4288,14 @@
       </c>
       <c r="E72" s="9">
         <f t="shared" si="12"/>
-        <v>6800</v>
+        <v>81600</v>
       </c>
       <c r="H72" s="4">
         <v>93150</v>
       </c>
       <c r="I72" s="4">
         <f>E72*1.5</f>
-        <v>10200</v>
+        <v>122400</v>
       </c>
       <c r="J72" s="4" t="s">
         <v>133</v>
@@ -4322,7 +4322,7 @@
       </c>
       <c r="E73" s="9">
         <f t="shared" si="12"/>
-        <v>6800</v>
+        <v>81600</v>
       </c>
       <c r="F73" s="4">
         <v>0</v>
@@ -4335,7 +4335,7 @@
       </c>
       <c r="I73" s="4">
         <f>E73*3</f>
-        <v>20400</v>
+        <v>244800</v>
       </c>
       <c r="K73" s="4">
         <v>6800</v>
@@ -4359,7 +4359,7 @@
       </c>
       <c r="E74" s="9">
         <f t="shared" si="12"/>
-        <v>6500</v>
+        <v>78000</v>
       </c>
       <c r="F74" s="4">
         <v>0</v>
@@ -4372,7 +4372,7 @@
       </c>
       <c r="I74" s="4">
         <f>E74*3</f>
-        <v>19500</v>
+        <v>234000</v>
       </c>
       <c r="K74" s="8">
         <v>6500</v>
@@ -4854,8 +4854,8 @@
         <v>6</v>
       </c>
       <c r="E91" s="9">
-        <f t="shared" ref="E91:E92" si="15">K91</f>
-        <v>6500</v>
+        <f t="shared" ref="E91:E92" si="15">K91*12</f>
+        <v>78000</v>
       </c>
       <c r="F91" s="4">
         <v>39000</v>
@@ -4885,7 +4885,7 @@
       </c>
       <c r="E92" s="9">
         <f t="shared" si="15"/>
-        <v>6500</v>
+        <v>78000</v>
       </c>
       <c r="F92" s="4">
         <v>39000</v>
@@ -5199,8 +5199,8 @@
         <v>6</v>
       </c>
       <c r="E103" s="9">
-        <f>K103</f>
-        <v>12500</v>
+        <f>K103*12</f>
+        <v>150000</v>
       </c>
       <c r="H103" s="4">
         <v>150000</v>
@@ -5448,8 +5448,8 @@
         <v>6</v>
       </c>
       <c r="E112" s="9">
-        <f t="shared" ref="E112:E115" si="18">K112</f>
-        <v>4300</v>
+        <f t="shared" ref="E112:E115" si="18">K112*12</f>
+        <v>51600</v>
       </c>
       <c r="H112" s="4">
         <v>51600</v>
@@ -5476,7 +5476,7 @@
       </c>
       <c r="E113" s="9">
         <f t="shared" si="18"/>
-        <v>9250</v>
+        <v>111000</v>
       </c>
       <c r="F113" s="4">
         <v>0</v>
@@ -5512,7 +5512,7 @@
       </c>
       <c r="E114" s="9">
         <f t="shared" si="18"/>
-        <v>7916</v>
+        <v>94992</v>
       </c>
       <c r="H114">
         <f>K114*12</f>
@@ -5540,7 +5540,7 @@
       </c>
       <c r="E115" s="9">
         <f t="shared" si="18"/>
-        <v>7916</v>
+        <v>94992</v>
       </c>
       <c r="H115" s="4">
         <v>103000</v>
@@ -5596,15 +5596,15 @@
         <v>6</v>
       </c>
       <c r="E117" s="9">
-        <f>K117</f>
-        <v>7916</v>
+        <f>K117*12</f>
+        <v>94992</v>
       </c>
       <c r="H117" s="4">
         <v>110000</v>
       </c>
       <c r="I117" s="4">
         <f>E117</f>
-        <v>7916</v>
+        <v>94992</v>
       </c>
       <c r="K117" s="4">
         <v>7916</v>
@@ -5881,8 +5881,8 @@
         <v>36</v>
       </c>
       <c r="E127" s="9">
-        <f t="shared" ref="E127:E132" si="21">K127</f>
-        <v>15000</v>
+        <f t="shared" ref="E127:E132" si="21">K127*12</f>
+        <v>180000</v>
       </c>
       <c r="H127">
         <f>K127*12</f>
@@ -5917,7 +5917,7 @@
       </c>
       <c r="E128" s="9">
         <f t="shared" si="21"/>
-        <v>8000</v>
+        <v>96000</v>
       </c>
       <c r="F128" s="4">
         <v>0</v>
@@ -5953,7 +5953,7 @@
       </c>
       <c r="E129" s="9">
         <f t="shared" si="21"/>
-        <v>6500</v>
+        <v>78000</v>
       </c>
       <c r="H129">
         <f>K129*12</f>
@@ -5981,7 +5981,7 @@
       </c>
       <c r="E130" s="9">
         <f t="shared" si="21"/>
-        <v>5500</v>
+        <v>66000</v>
       </c>
       <c r="F130" s="4">
         <v>0</v>
@@ -6020,7 +6020,7 @@
       </c>
       <c r="E131" s="9">
         <f t="shared" si="21"/>
-        <v>5500</v>
+        <v>66000</v>
       </c>
       <c r="F131" s="4">
         <v>0</v>
@@ -6059,7 +6059,7 @@
       </c>
       <c r="E132" s="9">
         <f t="shared" si="21"/>
-        <v>5000</v>
+        <v>60000</v>
       </c>
       <c r="H132">
         <f>K132*12</f>
@@ -6239,8 +6239,8 @@
         <v>6</v>
       </c>
       <c r="E138" s="9">
-        <f t="shared" ref="E138:E139" si="23">K138</f>
-        <v>7100</v>
+        <f t="shared" ref="E138:E139" si="23">K138*12</f>
+        <v>85200</v>
       </c>
       <c r="F138" s="4">
         <v>25000</v>
@@ -6280,7 +6280,7 @@
       </c>
       <c r="E139" s="9">
         <f t="shared" si="23"/>
-        <v>5417</v>
+        <v>65004</v>
       </c>
       <c r="H139">
         <f>K139*12</f>
@@ -6487,8 +6487,8 @@
         <v>219</v>
       </c>
       <c r="E146" s="9">
-        <f t="shared" ref="E146:E148" si="25">K146</f>
-        <v>5500</v>
+        <f t="shared" ref="E146:E148" si="25">K146*12</f>
+        <v>66000</v>
       </c>
       <c r="F146" s="4">
         <v>0</v>
@@ -6502,7 +6502,7 @@
       </c>
       <c r="I146" s="4">
         <f t="shared" ref="I146:I147" si="26">E146*4</f>
-        <v>22000</v>
+        <v>264000</v>
       </c>
       <c r="K146" s="4">
         <v>5500</v>
@@ -6526,14 +6526,14 @@
       </c>
       <c r="E147" s="9">
         <f t="shared" si="25"/>
-        <v>5400</v>
+        <v>64800</v>
       </c>
       <c r="H147" s="4">
         <v>90000</v>
       </c>
       <c r="I147" s="4">
         <f t="shared" si="26"/>
-        <v>21600</v>
+        <v>259200</v>
       </c>
       <c r="K147" s="9">
         <v>5400</v>
@@ -6557,7 +6557,7 @@
       </c>
       <c r="E148" s="9">
         <f t="shared" si="25"/>
-        <v>5000</v>
+        <v>60000</v>
       </c>
       <c r="H148">
         <f>K148*12</f>
@@ -6565,7 +6565,7 @@
       </c>
       <c r="I148" s="4">
         <f>E148*4</f>
-        <v>20000</v>
+        <v>240000</v>
       </c>
       <c r="J148" s="4" t="s">
         <v>242</v>
@@ -6729,8 +6729,8 @@
         <v>169</v>
       </c>
       <c r="E154" s="9">
-        <f t="shared" ref="E154:E159" si="28">K154</f>
-        <v>5400</v>
+        <f t="shared" ref="E154:E159" si="28">K154*12</f>
+        <v>64800</v>
       </c>
       <c r="H154">
         <f>K154*12</f>
@@ -6738,7 +6738,7 @@
       </c>
       <c r="I154" s="4">
         <f t="shared" ref="I154:I155" si="29">E154*3.5</f>
-        <v>18900</v>
+        <v>226800</v>
       </c>
       <c r="J154" s="4" t="s">
         <v>222</v>
@@ -6765,14 +6765,14 @@
       </c>
       <c r="E155" s="9">
         <f t="shared" si="28"/>
-        <v>5700</v>
+        <v>68400</v>
       </c>
       <c r="H155" s="4">
         <v>84300</v>
       </c>
       <c r="I155" s="4">
         <f t="shared" si="29"/>
-        <v>19950</v>
+        <v>239400</v>
       </c>
       <c r="K155" s="4">
         <v>5700</v>
@@ -6796,7 +6796,7 @@
       </c>
       <c r="E156" s="9">
         <f t="shared" si="28"/>
-        <v>5000</v>
+        <v>60000</v>
       </c>
       <c r="F156" s="4">
         <v>0</v>
@@ -6810,7 +6810,7 @@
       </c>
       <c r="I156" s="4">
         <f>E156*3.5</f>
-        <v>17500</v>
+        <v>210000</v>
       </c>
       <c r="K156" s="9">
         <v>5000</v>
@@ -6834,7 +6834,7 @@
       </c>
       <c r="E157" s="9">
         <f t="shared" si="28"/>
-        <v>5000</v>
+        <v>60000</v>
       </c>
       <c r="H157" s="4">
         <v>60000</v>
@@ -6867,7 +6867,7 @@
       </c>
       <c r="E158" s="9">
         <f t="shared" si="28"/>
-        <v>6200</v>
+        <v>74400</v>
       </c>
       <c r="H158" s="4">
         <v>94700</v>
@@ -6900,7 +6900,7 @@
       </c>
       <c r="E159" s="9">
         <f t="shared" si="28"/>
-        <v>5000</v>
+        <v>60000</v>
       </c>
       <c r="F159" s="4">
         <v>0</v>
@@ -6990,8 +6990,8 @@
         <v>6</v>
       </c>
       <c r="E162" s="9">
-        <f>K162</f>
-        <v>4200</v>
+        <f>K162*12</f>
+        <v>50400</v>
       </c>
       <c r="H162">
         <f>K162*12</f>
@@ -7094,15 +7094,15 @@
         <v>14</v>
       </c>
       <c r="E166" s="9">
-        <f t="shared" ref="E166:E169" si="31">K166</f>
-        <v>4000</v>
+        <f t="shared" ref="E166:E169" si="31">K166*12</f>
+        <v>48000</v>
       </c>
       <c r="H166" s="4">
         <v>48000</v>
       </c>
       <c r="I166" s="4">
         <f>E166*2</f>
-        <v>8000</v>
+        <v>96000</v>
       </c>
       <c r="K166" s="4">
         <v>4000</v>
@@ -7123,7 +7123,7 @@
       </c>
       <c r="E167" s="9">
         <f t="shared" si="31"/>
-        <v>4000</v>
+        <v>48000</v>
       </c>
       <c r="H167" s="4">
         <v>48000</v>
@@ -7147,7 +7147,7 @@
       </c>
       <c r="E168" s="9">
         <f t="shared" si="31"/>
-        <v>4000</v>
+        <v>48000</v>
       </c>
       <c r="H168">
         <f>K168*12</f>
@@ -7172,7 +7172,7 @@
       </c>
       <c r="E169" s="9">
         <f t="shared" si="31"/>
-        <v>4000</v>
+        <v>48000</v>
       </c>
       <c r="H169">
         <f>K169*12</f>
@@ -7274,8 +7274,8 @@
         <v>6</v>
       </c>
       <c r="E173" s="9">
-        <f t="shared" ref="E173:E180" si="33">K173</f>
-        <v>9750</v>
+        <f t="shared" ref="E173:E180" si="33">K173*12</f>
+        <v>117000</v>
       </c>
       <c r="F173" s="4">
         <v>25000</v>
@@ -7312,7 +7312,7 @@
       </c>
       <c r="E174" s="9">
         <f t="shared" si="33"/>
-        <v>7900</v>
+        <v>94800</v>
       </c>
       <c r="F174" s="4">
         <v>45000</v>
@@ -7325,7 +7325,7 @@
       </c>
       <c r="I174" s="4">
         <f>E175*2</f>
-        <v>15200</v>
+        <v>182400</v>
       </c>
       <c r="J174" s="4" t="s">
         <v>93</v>
@@ -7349,7 +7349,7 @@
       </c>
       <c r="E175" s="9">
         <f t="shared" si="33"/>
-        <v>7600</v>
+        <v>91200</v>
       </c>
       <c r="F175" s="4">
         <v>30000</v>
@@ -7386,7 +7386,7 @@
       </c>
       <c r="E176" s="9">
         <f t="shared" si="33"/>
-        <v>7600</v>
+        <v>91200</v>
       </c>
       <c r="F176" s="4">
         <v>35000</v>
@@ -7423,7 +7423,7 @@
       </c>
       <c r="E177" s="9">
         <f t="shared" si="33"/>
-        <v>7000</v>
+        <v>84000</v>
       </c>
       <c r="F177" s="4">
         <v>35000</v>
@@ -7460,7 +7460,7 @@
       </c>
       <c r="E178" s="9">
         <f t="shared" si="33"/>
-        <v>7000</v>
+        <v>84000</v>
       </c>
       <c r="F178" s="4">
         <v>35000</v>
@@ -7497,7 +7497,7 @@
       </c>
       <c r="E179" s="9">
         <f t="shared" si="33"/>
-        <v>6500</v>
+        <v>78000</v>
       </c>
       <c r="F179" s="4">
         <v>0</v>
@@ -7534,7 +7534,7 @@
       </c>
       <c r="E180" s="9">
         <f t="shared" si="33"/>
-        <v>6000</v>
+        <v>72000</v>
       </c>
       <c r="F180" s="4">
         <v>0</v>
@@ -7591,8 +7591,8 @@
         <v>488</v>
       </c>
       <c r="E182" s="9">
-        <f t="shared" ref="E182:E185" si="35">K182</f>
-        <v>9441.6666666666661</v>
+        <f t="shared" ref="E182:E185" si="35">K182*12</f>
+        <v>113300</v>
       </c>
       <c r="F182" s="4">
         <v>10200</v>
@@ -7624,7 +7624,7 @@
       </c>
       <c r="E183" s="9">
         <f t="shared" si="35"/>
-        <v>6750</v>
+        <v>81000</v>
       </c>
       <c r="F183" s="4">
         <v>0</v>
@@ -7661,7 +7661,7 @@
       </c>
       <c r="E184" s="9">
         <f t="shared" si="35"/>
-        <v>6600</v>
+        <v>79200</v>
       </c>
       <c r="F184" s="4">
         <v>0</v>
@@ -7674,7 +7674,7 @@
       </c>
       <c r="I184" s="4">
         <f>E184*1.5</f>
-        <v>9900</v>
+        <v>118800</v>
       </c>
       <c r="K184" s="4">
         <v>6600</v>
@@ -7695,7 +7695,7 @@
       </c>
       <c r="E185" s="9">
         <f t="shared" si="35"/>
-        <v>5000</v>
+        <v>60000</v>
       </c>
       <c r="H185">
         <f>K185*12</f>
@@ -7842,8 +7842,8 @@
         <v>6</v>
       </c>
       <c r="E191" s="9">
-        <f t="shared" ref="E191:E192" si="37">K191</f>
-        <v>7000</v>
+        <f t="shared" ref="E191:E192" si="37">K191*12</f>
+        <v>84000</v>
       </c>
       <c r="H191" s="4">
         <v>117500</v>
@@ -7873,7 +7873,7 @@
       </c>
       <c r="E192" s="9">
         <f t="shared" si="37"/>
-        <v>7000</v>
+        <v>84000</v>
       </c>
       <c r="H192">
         <f>K192*12</f>
@@ -7881,7 +7881,7 @@
       </c>
       <c r="I192" s="4">
         <f>E192*3</f>
-        <v>21000</v>
+        <v>252000</v>
       </c>
       <c r="J192" s="4" t="s">
         <v>131</v>
@@ -8198,8 +8198,8 @@
         <v>6</v>
       </c>
       <c r="E205" s="9">
-        <f t="shared" ref="E205:E208" si="39">K205</f>
-        <v>7000</v>
+        <f t="shared" ref="E205:E208" si="39">K205*12</f>
+        <v>84000</v>
       </c>
       <c r="H205">
         <f>K205*12</f>
@@ -8224,7 +8224,7 @@
       </c>
       <c r="E206" s="9">
         <f t="shared" si="39"/>
-        <v>6250</v>
+        <v>75000</v>
       </c>
       <c r="F206" s="4">
         <v>0</v>
@@ -8260,7 +8260,7 @@
       </c>
       <c r="E207" s="9">
         <f t="shared" si="39"/>
-        <v>6250</v>
+        <v>75000</v>
       </c>
       <c r="G207" s="4">
         <v>16000</v>
@@ -8294,7 +8294,7 @@
       </c>
       <c r="E208" s="9">
         <f t="shared" si="39"/>
-        <v>5833</v>
+        <v>69996</v>
       </c>
       <c r="F208" s="4">
         <v>0</v>
@@ -8449,8 +8449,8 @@
         <v>6</v>
       </c>
       <c r="E214" s="9">
-        <f t="shared" ref="E214:E216" si="41">K214</f>
-        <v>10000</v>
+        <f t="shared" ref="E214:E216" si="41">K214*12</f>
+        <v>120000</v>
       </c>
       <c r="F214" s="4">
         <v>145000</v>
@@ -8463,7 +8463,7 @@
       </c>
       <c r="I214" s="4">
         <f>E214*3</f>
-        <v>30000</v>
+        <v>360000</v>
       </c>
       <c r="K214" s="9">
         <v>10000</v>
@@ -8484,7 +8484,7 @@
       </c>
       <c r="E215" s="9">
         <f t="shared" si="41"/>
-        <v>7167</v>
+        <v>86004</v>
       </c>
       <c r="F215" s="4">
         <v>70000</v>
@@ -8518,7 +8518,7 @@
       </c>
       <c r="E216" s="9">
         <f t="shared" si="41"/>
-        <v>7166</v>
+        <v>85992</v>
       </c>
       <c r="F216" s="4">
         <v>70000</v>
@@ -8671,8 +8671,8 @@
         <v>81</v>
       </c>
       <c r="E222" s="9">
-        <f t="shared" ref="E222:E224" si="43">K222</f>
-        <v>8400</v>
+        <f t="shared" ref="E222:E224" si="43">K222*12</f>
+        <v>100800</v>
       </c>
       <c r="F222" s="4">
         <v>0</v>
@@ -8705,7 +8705,7 @@
       </c>
       <c r="E223" s="9">
         <f t="shared" si="43"/>
-        <v>6000</v>
+        <v>72000</v>
       </c>
       <c r="F223" s="4">
         <v>0</v>
@@ -8741,7 +8741,7 @@
       </c>
       <c r="E224" s="9">
         <f t="shared" si="43"/>
-        <v>5500</v>
+        <v>66000</v>
       </c>
       <c r="F224" s="4">
         <v>0</v>
@@ -8754,7 +8754,7 @@
       </c>
       <c r="I224" s="4">
         <f>E224*3</f>
-        <v>16500</v>
+        <v>198000</v>
       </c>
       <c r="J224" s="4" t="s">
         <v>218</v>
@@ -9303,8 +9303,8 @@
         <v>6</v>
       </c>
       <c r="E246" s="9">
-        <f t="shared" ref="E246:E248" si="45">K246</f>
-        <v>8000</v>
+        <f t="shared" ref="E246:E248" si="45">K246*12</f>
+        <v>96000</v>
       </c>
       <c r="F246" s="4">
         <v>36920</v>
@@ -9341,7 +9341,7 @@
       </c>
       <c r="E247" s="9">
         <f t="shared" si="45"/>
-        <v>6500</v>
+        <v>78000</v>
       </c>
       <c r="F247" s="4">
         <v>36920</v>
@@ -9378,7 +9378,7 @@
       </c>
       <c r="E248" s="9">
         <f t="shared" si="45"/>
-        <v>5500</v>
+        <v>66000</v>
       </c>
       <c r="H248">
         <f>K248*12</f>
@@ -9386,7 +9386,7 @@
       </c>
       <c r="I248" s="4">
         <f>E248*2</f>
-        <v>11000</v>
+        <v>132000</v>
       </c>
       <c r="K248" s="4">
         <v>5500</v>
@@ -9622,8 +9622,8 @@
         <v>309</v>
       </c>
       <c r="E258" s="9">
-        <f>K258</f>
-        <v>4000</v>
+        <f>K258*12</f>
+        <v>48000</v>
       </c>
       <c r="F258" s="4">
         <v>0</v>
@@ -9636,7 +9636,7 @@
       </c>
       <c r="I258" s="4">
         <f>E258*1.5</f>
-        <v>6000</v>
+        <v>72000</v>
       </c>
       <c r="J258" s="4" t="s">
         <v>310</v>
@@ -9782,8 +9782,8 @@
         <v>6</v>
       </c>
       <c r="E264" s="9">
-        <f>K264</f>
-        <v>6000</v>
+        <f>K264*12</f>
+        <v>72000</v>
       </c>
       <c r="F264" s="4" t="s">
         <v>165</v>
@@ -10073,8 +10073,8 @@
         <v>54</v>
       </c>
       <c r="E275" s="9">
-        <f>K275</f>
-        <v>10000</v>
+        <f>K275*12</f>
+        <v>120000</v>
       </c>
       <c r="H275" s="4">
         <v>120000</v>
@@ -10247,8 +10247,8 @@
         <v>6</v>
       </c>
       <c r="E282" s="9">
-        <f t="shared" ref="E282:E287" si="50">K282</f>
-        <v>7916.666666666667</v>
+        <f t="shared" ref="E282:E287" si="50">K282*12</f>
+        <v>95000</v>
       </c>
       <c r="F282" s="4">
         <v>50000</v>
@@ -10279,7 +10279,7 @@
       </c>
       <c r="E283" s="9">
         <f t="shared" si="50"/>
-        <v>5416.666666666667</v>
+        <v>65000</v>
       </c>
       <c r="F283" s="4">
         <v>5000</v>
@@ -10317,7 +10317,7 @@
       </c>
       <c r="E284" s="9">
         <f t="shared" si="50"/>
-        <v>8750</v>
+        <v>105000</v>
       </c>
       <c r="F284" s="4">
         <v>53000</v>
@@ -10355,7 +10355,7 @@
       </c>
       <c r="E285" s="9">
         <f t="shared" si="50"/>
-        <v>8750</v>
+        <v>105000</v>
       </c>
       <c r="F285" s="4">
         <v>53000</v>
@@ -10393,7 +10393,7 @@
       </c>
       <c r="E286" s="9">
         <f t="shared" si="50"/>
-        <v>7900</v>
+        <v>94800</v>
       </c>
       <c r="F286" s="4">
         <v>50000</v>
@@ -10427,7 +10427,7 @@
       </c>
       <c r="E287" s="9">
         <f t="shared" si="50"/>
-        <v>5833</v>
+        <v>69996</v>
       </c>
       <c r="F287" s="4">
         <v>0</v>
@@ -10504,8 +10504,8 @@
         <v>6</v>
       </c>
       <c r="E290" s="9">
-        <f t="shared" ref="E290:E291" si="52">K290</f>
-        <v>5417</v>
+        <f t="shared" ref="E290:E291" si="52">K290*12</f>
+        <v>65004</v>
       </c>
       <c r="F290" s="4">
         <v>0</v>
@@ -10535,7 +10535,7 @@
       </c>
       <c r="E291" s="9">
         <f t="shared" si="52"/>
-        <v>5417</v>
+        <v>65004</v>
       </c>
       <c r="F291" s="4">
         <v>5000</v>
@@ -10592,8 +10592,8 @@
         <v>6</v>
       </c>
       <c r="E293" s="9">
-        <f>K293</f>
-        <v>5000</v>
+        <f>K293*12</f>
+        <v>60000</v>
       </c>
       <c r="F293" s="4">
         <v>10000</v>
@@ -10731,8 +10731,8 @@
         <v>322</v>
       </c>
       <c r="E298" s="9">
-        <f t="shared" ref="E298:E299" si="54">K298</f>
-        <v>3700</v>
+        <f t="shared" ref="E298:E299" si="54">K298*12</f>
+        <v>44400</v>
       </c>
       <c r="F298" s="4">
         <v>0</v>
@@ -10745,7 +10745,7 @@
       </c>
       <c r="I298" s="4">
         <f>E298*3</f>
-        <v>11100</v>
+        <v>133200</v>
       </c>
       <c r="K298" s="9">
         <v>3700</v>
@@ -10766,7 +10766,7 @@
       </c>
       <c r="E299" s="9">
         <f t="shared" si="54"/>
-        <v>25000</v>
+        <v>300000</v>
       </c>
       <c r="F299" s="4">
         <v>0</v>
@@ -10858,8 +10858,8 @@
         <v>6</v>
       </c>
       <c r="E302" s="9">
-        <f>K302</f>
-        <v>30000</v>
+        <f>K302*12</f>
+        <v>360000</v>
       </c>
       <c r="H302">
         <f>K302*12+G302+F302</f>
@@ -10919,8 +10919,8 @@
         <v>6</v>
       </c>
       <c r="E304" s="9">
-        <f>K304</f>
-        <v>6666</v>
+        <f>K304*12</f>
+        <v>79992</v>
       </c>
       <c r="F304" s="4">
         <v>0</v>
@@ -11003,8 +11003,8 @@
         <v>6</v>
       </c>
       <c r="E307" s="9">
-        <f>K307</f>
-        <v>5833.33</v>
+        <f>K307*12</f>
+        <v>69999.959999999992</v>
       </c>
       <c r="H307" s="4">
         <v>70000</v>
@@ -11135,8 +11135,8 @@
         <v>6</v>
       </c>
       <c r="E312" s="9">
-        <f t="shared" ref="E312:E314" si="57">K312</f>
-        <v>5833</v>
+        <f t="shared" ref="E312:E314" si="57">K312*12</f>
+        <v>69996</v>
       </c>
       <c r="F312" s="4">
         <v>0</v>
@@ -11172,7 +11172,7 @@
       </c>
       <c r="E313" s="9">
         <f t="shared" si="57"/>
-        <v>5667</v>
+        <v>68004</v>
       </c>
       <c r="F313" s="4">
         <v>0</v>
@@ -11208,7 +11208,7 @@
       </c>
       <c r="E314" s="9">
         <f t="shared" si="57"/>
-        <v>5416</v>
+        <v>64992</v>
       </c>
       <c r="F314" s="4">
         <v>0</v>
@@ -11351,8 +11351,8 @@
         <v>6</v>
       </c>
       <c r="E319" s="9">
-        <f>K319</f>
-        <v>5000</v>
+        <f>K319*12</f>
+        <v>60000</v>
       </c>
       <c r="F319" s="4">
         <v>0</v>
@@ -11362,7 +11362,7 @@
       </c>
       <c r="I319" s="4">
         <f>E319*1.5</f>
-        <v>7500</v>
+        <v>90000</v>
       </c>
       <c r="J319" s="4" t="s">
         <v>248</v>
@@ -11436,8 +11436,8 @@
         <v>6</v>
       </c>
       <c r="E322" s="9">
-        <f t="shared" ref="E322:E323" si="59">K322</f>
-        <v>9333</v>
+        <f t="shared" ref="E322:E323" si="59">K322*12</f>
+        <v>111996</v>
       </c>
       <c r="F322" s="4">
         <v>50000</v>
@@ -11475,7 +11475,7 @@
       </c>
       <c r="E323" s="9">
         <f t="shared" si="59"/>
-        <v>9333</v>
+        <v>111996</v>
       </c>
       <c r="F323" s="4">
         <v>50000</v>
@@ -11760,8 +11760,8 @@
         <v>256</v>
       </c>
       <c r="E334" s="9">
-        <f t="shared" ref="E334:E336" si="61">K334</f>
-        <v>5000</v>
+        <f t="shared" ref="E334:E336" si="61">K334*12</f>
+        <v>60000</v>
       </c>
       <c r="H334">
         <f>K334*12</f>
@@ -11790,7 +11790,7 @@
       </c>
       <c r="E335" s="9">
         <f t="shared" si="61"/>
-        <v>6250</v>
+        <v>75000</v>
       </c>
       <c r="F335" s="4">
         <v>0</v>
@@ -11826,7 +11826,7 @@
       </c>
       <c r="E336" s="9">
         <f t="shared" si="61"/>
-        <v>3900</v>
+        <v>46800</v>
       </c>
       <c r="H336">
         <f>K336*12</f>
@@ -11834,7 +11834,7 @@
       </c>
       <c r="I336" s="4">
         <f>E336*4</f>
-        <v>15600</v>
+        <v>187200</v>
       </c>
       <c r="K336" s="4">
         <v>3900</v>
@@ -11901,8 +11901,8 @@
         <v>6</v>
       </c>
       <c r="E339" s="9">
-        <f t="shared" ref="E339:E340" si="62">K339</f>
-        <v>8500</v>
+        <f t="shared" ref="E339:E340" si="62">K339*12</f>
+        <v>102000</v>
       </c>
       <c r="F339" s="4">
         <v>20000</v>
@@ -11939,7 +11939,7 @@
       </c>
       <c r="E340" s="9">
         <f t="shared" si="62"/>
-        <v>8000</v>
+        <v>96000</v>
       </c>
       <c r="H340" s="4">
         <v>96000</v>
@@ -11989,8 +11989,8 @@
         <v>6</v>
       </c>
       <c r="E342" s="9">
-        <f t="shared" ref="E342:E353" si="63">K342</f>
-        <v>6000</v>
+        <f t="shared" ref="E342:E353" si="63">K342*12</f>
+        <v>72000</v>
       </c>
       <c r="F342" s="4">
         <v>0</v>
@@ -12004,7 +12004,7 @@
       </c>
       <c r="I342" s="4">
         <f>2*E342</f>
-        <v>12000</v>
+        <v>144000</v>
       </c>
       <c r="K342" s="9">
         <v>6000</v>
@@ -12025,7 +12025,7 @@
       </c>
       <c r="E343" s="9">
         <f t="shared" si="63"/>
-        <v>5678</v>
+        <v>68136</v>
       </c>
       <c r="H343">
         <f>K343*12</f>
@@ -12033,7 +12033,7 @@
       </c>
       <c r="I343" s="4">
         <f>3*E343</f>
-        <v>17034</v>
+        <v>204408</v>
       </c>
       <c r="J343" s="4" t="s">
         <v>191</v>
@@ -12057,7 +12057,7 @@
       </c>
       <c r="E344" s="9">
         <f t="shared" si="63"/>
-        <v>5400</v>
+        <v>64800</v>
       </c>
       <c r="H344">
         <f>K344*12</f>
@@ -12065,7 +12065,7 @@
       </c>
       <c r="I344" s="4">
         <f>2*E344</f>
-        <v>10800</v>
+        <v>129600</v>
       </c>
       <c r="K344" s="4">
         <v>5400</v>
@@ -12086,7 +12086,7 @@
       </c>
       <c r="E345" s="9">
         <f t="shared" si="63"/>
-        <v>5200</v>
+        <v>62400</v>
       </c>
       <c r="H345">
         <f>K345*12</f>
@@ -12111,7 +12111,7 @@
       </c>
       <c r="E346" s="9">
         <f t="shared" si="63"/>
-        <v>4800</v>
+        <v>57600</v>
       </c>
       <c r="H346">
         <f>K346*12</f>
@@ -12136,14 +12136,14 @@
       </c>
       <c r="E347" s="9">
         <f t="shared" si="63"/>
-        <v>4800</v>
+        <v>57600</v>
       </c>
       <c r="H347" s="4">
         <v>62400</v>
       </c>
       <c r="I347" s="4">
         <f>E347*2</f>
-        <v>9600</v>
+        <v>115200</v>
       </c>
       <c r="J347" s="4" t="s">
         <v>266</v>
@@ -12167,7 +12167,7 @@
       </c>
       <c r="E348" s="9">
         <f t="shared" si="63"/>
-        <v>4800</v>
+        <v>57600</v>
       </c>
       <c r="H348">
         <f>K348*12</f>
@@ -12192,7 +12192,7 @@
       </c>
       <c r="E349" s="9">
         <f t="shared" si="63"/>
-        <v>4800</v>
+        <v>57600</v>
       </c>
       <c r="H349">
         <f>K349*12</f>
@@ -12200,7 +12200,7 @@
       </c>
       <c r="I349" s="4">
         <f t="shared" ref="I349:I353" si="64">2*E349</f>
-        <v>9600</v>
+        <v>115200</v>
       </c>
       <c r="K349" s="4">
         <v>4800</v>
@@ -12221,7 +12221,7 @@
       </c>
       <c r="E350" s="9">
         <f t="shared" si="63"/>
-        <v>4500</v>
+        <v>54000</v>
       </c>
       <c r="F350" s="4">
         <v>0</v>
@@ -12234,7 +12234,7 @@
       </c>
       <c r="I350" s="4">
         <f t="shared" si="64"/>
-        <v>9000</v>
+        <v>108000</v>
       </c>
       <c r="J350" s="4" t="s">
         <v>276</v>
@@ -12258,14 +12258,14 @@
       </c>
       <c r="E351" s="9">
         <f t="shared" si="63"/>
-        <v>4500</v>
+        <v>54000</v>
       </c>
       <c r="H351" s="4">
         <v>54000</v>
       </c>
       <c r="I351" s="4">
         <f t="shared" si="64"/>
-        <v>9000</v>
+        <v>108000</v>
       </c>
       <c r="J351" s="4" t="s">
         <v>278</v>
@@ -12289,7 +12289,7 @@
       </c>
       <c r="E352" s="9">
         <f t="shared" si="63"/>
-        <v>4200</v>
+        <v>50400</v>
       </c>
       <c r="F352" s="4" t="s">
         <v>283</v>
@@ -12303,7 +12303,7 @@
       </c>
       <c r="I352" s="4">
         <f t="shared" si="64"/>
-        <v>8400</v>
+        <v>100800</v>
       </c>
       <c r="J352" s="4" t="s">
         <v>284</v>
@@ -12327,7 +12327,7 @@
       </c>
       <c r="E353" s="9">
         <f t="shared" si="63"/>
-        <v>4000</v>
+        <v>48000</v>
       </c>
       <c r="F353" s="4">
         <v>0</v>
@@ -12341,7 +12341,7 @@
       </c>
       <c r="I353" s="4">
         <f t="shared" si="64"/>
-        <v>8000</v>
+        <v>96000</v>
       </c>
       <c r="J353" s="4" t="s">
         <v>303</v>
@@ -12389,15 +12389,15 @@
         <v>6</v>
       </c>
       <c r="E355" s="9">
-        <f t="shared" ref="E355:E358" si="65">K355</f>
-        <v>6600</v>
+        <f t="shared" ref="E355:E358" si="65">K355*12</f>
+        <v>79200</v>
       </c>
       <c r="H355" s="4">
         <v>96000</v>
       </c>
       <c r="I355" s="4">
         <f>2*E355</f>
-        <v>13200</v>
+        <v>158400</v>
       </c>
       <c r="J355" s="4" t="s">
         <v>140</v>
@@ -12421,7 +12421,7 @@
       </c>
       <c r="E356" s="9">
         <f t="shared" si="65"/>
-        <v>6500</v>
+        <v>78000</v>
       </c>
       <c r="F356" s="4">
         <v>21000</v>
@@ -12452,7 +12452,7 @@
       </c>
       <c r="E357" s="9">
         <f t="shared" si="65"/>
-        <v>5500</v>
+        <v>66000</v>
       </c>
       <c r="H357">
         <f>K357*12+F357</f>
@@ -12480,7 +12480,7 @@
       </c>
       <c r="E358" s="9">
         <f t="shared" si="65"/>
-        <v>5500</v>
+        <v>66000</v>
       </c>
       <c r="F358" s="4">
         <v>24750</v>
@@ -12561,8 +12561,8 @@
         <v>292</v>
       </c>
       <c r="E361" s="9">
-        <f>K361</f>
-        <v>4100</v>
+        <f>K361*12</f>
+        <v>49200</v>
       </c>
       <c r="H361">
         <f>K361*12+F361</f>
@@ -12610,8 +12610,8 @@
         <v>6</v>
       </c>
       <c r="E363" s="9">
-        <f t="shared" ref="E363:E370" si="67">K363</f>
-        <v>9628</v>
+        <f t="shared" ref="E363:E370" si="67">K363*12</f>
+        <v>115536</v>
       </c>
       <c r="F363" s="4">
         <v>0</v>
@@ -12624,7 +12624,7 @@
       </c>
       <c r="I363" s="4">
         <f t="shared" ref="I363:I369" si="68">E363*3</f>
-        <v>28884</v>
+        <v>346608</v>
       </c>
       <c r="J363" s="4" t="s">
         <v>63</v>
@@ -12648,7 +12648,7 @@
       </c>
       <c r="E364" s="9">
         <f t="shared" si="67"/>
-        <v>9000</v>
+        <v>108000</v>
       </c>
       <c r="G364" s="4" t="s">
         <v>72</v>
@@ -12658,7 +12658,7 @@
       </c>
       <c r="I364" s="4">
         <f t="shared" si="68"/>
-        <v>27000</v>
+        <v>324000</v>
       </c>
       <c r="J364" s="4" t="s">
         <v>73</v>
@@ -12682,7 +12682,7 @@
       </c>
       <c r="E365" s="9">
         <f t="shared" si="67"/>
-        <v>8986</v>
+        <v>107832</v>
       </c>
       <c r="F365" s="4">
         <v>0</v>
@@ -12695,7 +12695,7 @@
       </c>
       <c r="I365" s="4">
         <f t="shared" si="68"/>
-        <v>26958</v>
+        <v>323496</v>
       </c>
       <c r="K365" s="4">
         <v>8986</v>
@@ -12716,7 +12716,7 @@
       </c>
       <c r="E366" s="9">
         <f t="shared" si="67"/>
-        <v>9625</v>
+        <v>115500</v>
       </c>
       <c r="G366" s="4" t="s">
         <v>29</v>
@@ -12726,7 +12726,7 @@
       </c>
       <c r="I366" s="4">
         <f t="shared" si="68"/>
-        <v>28875</v>
+        <v>346500</v>
       </c>
       <c r="K366" s="9">
         <f>115500/12</f>
@@ -12748,7 +12748,7 @@
       </c>
       <c r="E367" s="9">
         <f t="shared" si="67"/>
-        <v>9628</v>
+        <v>115536</v>
       </c>
       <c r="G367" s="4">
         <v>19256</v>
@@ -12758,7 +12758,7 @@
       </c>
       <c r="I367" s="4">
         <f t="shared" si="68"/>
-        <v>28884</v>
+        <v>346608</v>
       </c>
       <c r="J367" s="4" t="s">
         <v>62</v>
@@ -12782,7 +12782,7 @@
       </c>
       <c r="E368" s="9">
         <f t="shared" si="67"/>
-        <v>9000</v>
+        <v>108000</v>
       </c>
       <c r="G368" s="4">
         <v>18000</v>
@@ -12792,7 +12792,7 @@
       </c>
       <c r="I368" s="4">
         <f t="shared" si="68"/>
-        <v>27000</v>
+        <v>324000</v>
       </c>
       <c r="K368" s="4">
         <v>9000</v>
@@ -12813,7 +12813,7 @@
       </c>
       <c r="E369" s="9">
         <f t="shared" si="67"/>
-        <v>7770</v>
+        <v>93240</v>
       </c>
       <c r="F369" s="4" t="s">
         <v>95</v>
@@ -12826,7 +12826,7 @@
       </c>
       <c r="I369" s="4">
         <f t="shared" si="68"/>
-        <v>23310</v>
+        <v>279720</v>
       </c>
       <c r="J369" s="4" t="s">
         <v>96</v>
@@ -12850,7 +12850,7 @@
       </c>
       <c r="E370" s="9">
         <f t="shared" si="67"/>
-        <v>7770</v>
+        <v>93240</v>
       </c>
       <c r="F370" s="4">
         <v>0</v>
@@ -12863,7 +12863,7 @@
       </c>
       <c r="I370" s="4">
         <f>E370*3</f>
-        <v>23310</v>
+        <v>279720</v>
       </c>
       <c r="K370" s="9">
         <v>7770</v>
@@ -13027,8 +13027,8 @@
         <v>6</v>
       </c>
       <c r="E377" s="9">
-        <f>K377</f>
-        <v>20000</v>
+        <f>K377*12</f>
+        <v>240000</v>
       </c>
       <c r="H377">
         <f>K377*12+F377+G377</f>
@@ -13079,8 +13079,8 @@
         <v>347</v>
       </c>
       <c r="E379" s="9">
-        <f>K379</f>
-        <v>3000</v>
+        <f>K379*12</f>
+        <v>36000</v>
       </c>
       <c r="F379" s="4">
         <v>0</v>
@@ -13362,15 +13362,15 @@
         <v>74</v>
       </c>
       <c r="E390" s="9">
-        <f>K390</f>
-        <v>5500</v>
+        <f>K390*12</f>
+        <v>66000</v>
       </c>
       <c r="H390" s="4">
         <v>79000</v>
       </c>
       <c r="I390" s="4">
         <f>E390*4</f>
-        <v>22000</v>
+        <v>264000</v>
       </c>
       <c r="K390" s="4">
         <v>5500</v>
@@ -13414,8 +13414,8 @@
         <v>328</v>
       </c>
       <c r="E392" s="9">
-        <f t="shared" ref="E392:E393" si="70">K392</f>
-        <v>3600</v>
+        <f t="shared" ref="E392:E393" si="70">K392*12</f>
+        <v>43200</v>
       </c>
       <c r="H392" s="4">
         <v>66000</v>
@@ -13445,7 +13445,7 @@
       </c>
       <c r="E393" s="9">
         <f t="shared" si="70"/>
-        <v>2500</v>
+        <v>30000</v>
       </c>
       <c r="H393">
         <f>K393*12+F393+G393</f>
@@ -13453,7 +13453,7 @@
       </c>
       <c r="I393" s="4">
         <f>E393*3</f>
-        <v>7500</v>
+        <v>90000</v>
       </c>
       <c r="K393" s="9">
         <v>2500</v>
@@ -13590,8 +13590,8 @@
         <v>6</v>
       </c>
       <c r="E399" s="9">
-        <f t="shared" ref="E399:E400" si="72">K399</f>
-        <v>5800</v>
+        <f t="shared" ref="E399:E400" si="72">K399*12</f>
+        <v>69600</v>
       </c>
       <c r="F399" s="6">
         <v>0.1</v>
@@ -13626,7 +13626,7 @@
       </c>
       <c r="E400" s="9">
         <f t="shared" si="72"/>
-        <v>5000</v>
+        <v>60000</v>
       </c>
       <c r="F400" s="4">
         <v>0</v>
@@ -13639,7 +13639,7 @@
       </c>
       <c r="I400" s="4">
         <f>E400*1</f>
-        <v>5000</v>
+        <v>60000</v>
       </c>
       <c r="J400" s="4" t="s">
         <v>255</v>
@@ -13685,8 +13685,8 @@
         <v>169</v>
       </c>
       <c r="E402" s="9">
-        <f>K402</f>
-        <v>6000</v>
+        <f>K402*12</f>
+        <v>72000</v>
       </c>
       <c r="F402" s="4" t="s">
         <v>170</v>
@@ -13893,8 +13893,8 @@
         <v>6</v>
       </c>
       <c r="E410" s="9">
-        <f>K410</f>
-        <v>7000</v>
+        <f>K410*12</f>
+        <v>84000</v>
       </c>
       <c r="F410" s="4">
         <v>28000</v>
@@ -13974,8 +13974,8 @@
         <v>6</v>
       </c>
       <c r="E413" s="9">
-        <f>K413</f>
-        <v>5500</v>
+        <f>K413*12</f>
+        <v>66000</v>
       </c>
       <c r="F413" s="4" t="s">
         <v>210</v>
@@ -13986,7 +13986,7 @@
       </c>
       <c r="I413" s="4">
         <f>E413*3</f>
-        <v>16500</v>
+        <v>198000</v>
       </c>
       <c r="K413" s="4">
         <v>5500</v>
@@ -14105,8 +14105,8 @@
         <v>6</v>
       </c>
       <c r="E417" s="9">
-        <f>K417</f>
-        <v>7000</v>
+        <f>K417*12</f>
+        <v>84000</v>
       </c>
       <c r="F417" s="4">
         <v>50000</v>
@@ -14120,7 +14120,7 @@
       </c>
       <c r="I417" s="4">
         <f>2*E417</f>
-        <v>14000</v>
+        <v>168000</v>
       </c>
       <c r="J417" s="4" t="s">
         <v>115</v>
@@ -14191,8 +14191,8 @@
         <v>6</v>
       </c>
       <c r="E420" s="9">
-        <f t="shared" ref="E420:E436" si="76">K420</f>
-        <v>12000</v>
+        <f t="shared" ref="E420:E436" si="76">K420*12</f>
+        <v>144000</v>
       </c>
       <c r="H420" s="4">
         <f>K420*12</f>
@@ -14220,7 +14220,7 @@
       </c>
       <c r="E421" s="9">
         <f t="shared" si="76"/>
-        <v>8000</v>
+        <v>96000</v>
       </c>
       <c r="F421" s="4">
         <v>112000</v>
@@ -14233,7 +14233,7 @@
       </c>
       <c r="I421" s="4">
         <f t="shared" ref="I421:I426" si="77">2*E421</f>
-        <v>16000</v>
+        <v>192000</v>
       </c>
       <c r="K421" s="9">
         <v>8000</v>
@@ -14254,7 +14254,7 @@
       </c>
       <c r="E422" s="9">
         <f t="shared" si="76"/>
-        <v>7500</v>
+        <v>90000</v>
       </c>
       <c r="F422" s="4">
         <v>140000</v>
@@ -14264,7 +14264,7 @@
       </c>
       <c r="I422" s="4">
         <f t="shared" si="77"/>
-        <v>15000</v>
+        <v>180000</v>
       </c>
       <c r="J422" s="4" t="s">
         <v>100</v>
@@ -14288,7 +14288,7 @@
       </c>
       <c r="E423" s="9">
         <f t="shared" si="76"/>
-        <v>7500</v>
+        <v>90000</v>
       </c>
       <c r="F423" s="4">
         <v>140000</v>
@@ -14301,7 +14301,7 @@
       </c>
       <c r="I423" s="4">
         <f t="shared" si="77"/>
-        <v>15000</v>
+        <v>180000</v>
       </c>
       <c r="K423" s="9">
         <v>7500</v>
@@ -14322,7 +14322,7 @@
       </c>
       <c r="E424" s="9">
         <f t="shared" si="76"/>
-        <v>7200</v>
+        <v>86400</v>
       </c>
       <c r="F424" s="4">
         <v>77000</v>
@@ -14335,7 +14335,7 @@
       </c>
       <c r="I424" s="4">
         <f t="shared" si="77"/>
-        <v>14400</v>
+        <v>172800</v>
       </c>
       <c r="J424" s="4" t="s">
         <v>106</v>
@@ -14359,7 +14359,7 @@
       </c>
       <c r="E425" s="9">
         <f t="shared" si="76"/>
-        <v>6800</v>
+        <v>81600</v>
       </c>
       <c r="F425" s="4">
         <v>36000</v>
@@ -14372,7 +14372,7 @@
       </c>
       <c r="I425" s="4">
         <f t="shared" si="77"/>
-        <v>13600</v>
+        <v>163200</v>
       </c>
       <c r="K425" s="9">
         <v>6800</v>
@@ -14393,7 +14393,7 @@
       </c>
       <c r="E426" s="9">
         <f t="shared" si="76"/>
-        <v>6800</v>
+        <v>81600</v>
       </c>
       <c r="F426" s="4">
         <v>39200</v>
@@ -14406,7 +14406,7 @@
       </c>
       <c r="I426" s="4">
         <f t="shared" si="77"/>
-        <v>13600</v>
+        <v>163200</v>
       </c>
       <c r="J426" s="4" t="s">
         <v>134</v>
@@ -14430,7 +14430,7 @@
       </c>
       <c r="E427" s="9">
         <f t="shared" si="76"/>
-        <v>6500</v>
+        <v>78000</v>
       </c>
       <c r="F427" s="4">
         <v>170000</v>
@@ -14440,7 +14440,7 @@
       </c>
       <c r="I427" s="4">
         <f>2*E427</f>
-        <v>13000</v>
+        <v>156000</v>
       </c>
       <c r="K427" s="9">
         <v>6500</v>
@@ -14461,7 +14461,7 @@
       </c>
       <c r="E428" s="9">
         <f t="shared" si="76"/>
-        <v>6500</v>
+        <v>78000</v>
       </c>
       <c r="H428">
         <f>K428*12</f>
@@ -14486,7 +14486,7 @@
       </c>
       <c r="E429" s="9">
         <f t="shared" si="76"/>
-        <v>6500</v>
+        <v>78000</v>
       </c>
       <c r="F429" s="4">
         <v>9000</v>
@@ -14499,7 +14499,7 @@
       </c>
       <c r="I429" s="4">
         <f>E429*3</f>
-        <v>19500</v>
+        <v>234000</v>
       </c>
       <c r="J429" s="4" t="s">
         <v>144</v>
@@ -14523,7 +14523,7 @@
       </c>
       <c r="E430" s="9">
         <f t="shared" si="76"/>
-        <v>6200</v>
+        <v>74400</v>
       </c>
       <c r="F430" s="4">
         <f>49000/4</f>
@@ -14538,7 +14538,7 @@
       </c>
       <c r="I430" s="4">
         <f t="shared" ref="I430:I435" si="78">E430*2</f>
-        <v>12400</v>
+        <v>148800</v>
       </c>
       <c r="K430" s="9">
         <v>6200</v>
@@ -14559,7 +14559,7 @@
       </c>
       <c r="E431" s="9">
         <f t="shared" si="76"/>
-        <v>6200</v>
+        <v>74400</v>
       </c>
       <c r="F431" s="4" t="s">
         <v>155</v>
@@ -14572,7 +14572,7 @@
       </c>
       <c r="I431" s="4">
         <f t="shared" si="78"/>
-        <v>12400</v>
+        <v>148800</v>
       </c>
       <c r="J431" s="4" t="s">
         <v>156</v>
@@ -14596,7 +14596,7 @@
       </c>
       <c r="E432" s="9">
         <f t="shared" si="76"/>
-        <v>5800</v>
+        <v>69600</v>
       </c>
       <c r="F432" s="4" t="s">
         <v>132</v>
@@ -14609,7 +14609,7 @@
       </c>
       <c r="I432" s="4">
         <f t="shared" si="78"/>
-        <v>11600</v>
+        <v>139200</v>
       </c>
       <c r="K432" s="9">
         <v>5800</v>
@@ -14630,7 +14630,7 @@
       </c>
       <c r="E433" s="9">
         <f t="shared" si="76"/>
-        <v>5000</v>
+        <v>60000</v>
       </c>
       <c r="H433">
         <f>K433*12</f>
@@ -14656,7 +14656,7 @@
       </c>
       <c r="E434" s="9">
         <f t="shared" si="76"/>
-        <v>5000</v>
+        <v>60000</v>
       </c>
       <c r="H434">
         <f>K434*12</f>
@@ -14664,7 +14664,7 @@
       </c>
       <c r="I434" s="4">
         <f t="shared" si="78"/>
-        <v>10000</v>
+        <v>120000</v>
       </c>
       <c r="J434" s="4" t="s">
         <v>260</v>
@@ -14688,7 +14688,7 @@
       </c>
       <c r="E435" s="9">
         <f t="shared" si="76"/>
-        <v>4500</v>
+        <v>54000</v>
       </c>
       <c r="H435">
         <f>K435*12</f>
@@ -14696,7 +14696,7 @@
       </c>
       <c r="I435" s="4">
         <f t="shared" si="78"/>
-        <v>9000</v>
+        <v>108000</v>
       </c>
       <c r="J435" s="4" t="s">
         <v>275</v>
@@ -14720,7 +14720,7 @@
       </c>
       <c r="E436" s="9">
         <f t="shared" si="76"/>
-        <v>4500</v>
+        <v>54000</v>
       </c>
       <c r="H436">
         <f>K436*12</f>
@@ -14728,7 +14728,7 @@
       </c>
       <c r="I436" s="4">
         <f>E436*2</f>
-        <v>9000</v>
+        <v>108000</v>
       </c>
       <c r="K436" s="4">
         <v>4500</v>
@@ -15135,8 +15135,8 @@
         <v>6</v>
       </c>
       <c r="E453" s="9">
-        <f>K453</f>
-        <v>5200</v>
+        <f>K453*12</f>
+        <v>62400</v>
       </c>
       <c r="F453" s="4">
         <v>0</v>
@@ -15150,7 +15150,7 @@
       </c>
       <c r="I453" s="4">
         <f>E453*3</f>
-        <v>15600</v>
+        <v>187200</v>
       </c>
       <c r="K453" s="4">
         <v>5200</v>
@@ -15245,8 +15245,8 @@
         <v>320</v>
       </c>
       <c r="E457" s="9">
-        <f>K457</f>
-        <v>3800</v>
+        <f>K457*12</f>
+        <v>45600</v>
       </c>
       <c r="H457">
         <f>K457*12</f>
@@ -15297,8 +15297,8 @@
         <v>232</v>
       </c>
       <c r="E459" s="9">
-        <f t="shared" ref="E459:E460" si="80">K459</f>
-        <v>5200</v>
+        <f t="shared" ref="E459:E460" si="80">K459*12</f>
+        <v>62400</v>
       </c>
       <c r="F459" s="4" t="s">
         <v>233</v>
@@ -15331,7 +15331,7 @@
       </c>
       <c r="E460" s="9">
         <f t="shared" si="80"/>
-        <v>8333</v>
+        <v>99996</v>
       </c>
       <c r="F460" s="4">
         <v>20000</v>
@@ -15406,8 +15406,8 @@
         <v>6</v>
       </c>
       <c r="E463" s="9">
-        <f t="shared" ref="E463:E464" si="82">K463</f>
-        <v>7083</v>
+        <f t="shared" ref="E463:E464" si="82">K463*12</f>
+        <v>84996</v>
       </c>
       <c r="G463" s="4">
         <v>20000</v>
@@ -15438,7 +15438,7 @@
       </c>
       <c r="E464" s="9">
         <f t="shared" si="82"/>
-        <v>7083</v>
+        <v>84996</v>
       </c>
       <c r="G464" s="4">
         <v>10000</v>
@@ -15492,8 +15492,8 @@
         <v>6</v>
       </c>
       <c r="E466" s="9">
-        <f>K466</f>
-        <v>4800</v>
+        <f>K466*12</f>
+        <v>57600</v>
       </c>
       <c r="F466" s="4">
         <v>0</v>
@@ -15550,8 +15550,8 @@
         <v>217</v>
       </c>
       <c r="E468" s="9">
-        <f>K468</f>
-        <v>5500</v>
+        <f>K468*12</f>
+        <v>66000</v>
       </c>
       <c r="H468">
         <f>K468*12</f>
@@ -15559,7 +15559,7 @@
       </c>
       <c r="I468" s="4">
         <f>E468*1.25</f>
-        <v>6875</v>
+        <v>82500</v>
       </c>
       <c r="K468" s="4">
         <v>5500</v>
@@ -15603,8 +15603,8 @@
         <v>6</v>
       </c>
       <c r="E470" s="9">
-        <f>K470</f>
-        <v>5700</v>
+        <f>K470*12</f>
+        <v>68400</v>
       </c>
       <c r="H470">
         <f>K470*12</f>
@@ -15752,8 +15752,8 @@
         <v>6</v>
       </c>
       <c r="E476" s="9">
-        <f>K476</f>
-        <v>8333</v>
+        <f>K476*12</f>
+        <v>99996</v>
       </c>
       <c r="F476" s="4">
         <v>30000</v>
@@ -15867,8 +15867,8 @@
         <v>59</v>
       </c>
       <c r="E480" s="9">
-        <f t="shared" ref="E480:E481" si="84">K480</f>
-        <v>9800</v>
+        <f t="shared" ref="E480:E481" si="84">K480*12</f>
+        <v>117600</v>
       </c>
       <c r="F480" s="4">
         <v>20000</v>
@@ -15878,7 +15878,7 @@
       </c>
       <c r="I480" s="4">
         <f>E480*4</f>
-        <v>39200</v>
+        <v>470400</v>
       </c>
       <c r="K480" s="4">
         <v>9800</v>
@@ -15899,7 +15899,7 @@
       </c>
       <c r="E481" s="9">
         <f t="shared" si="84"/>
-        <v>4200</v>
+        <v>50400</v>
       </c>
       <c r="H481">
         <f>K481*12</f>
@@ -15999,8 +15999,8 @@
         <v>6</v>
       </c>
       <c r="E485" s="9">
-        <f t="shared" ref="E485:E488" si="86">K485</f>
-        <v>4000</v>
+        <f t="shared" ref="E485:E488" si="86">K485*12</f>
+        <v>48000</v>
       </c>
       <c r="H485">
         <f>K485*12</f>
@@ -16025,14 +16025,14 @@
       </c>
       <c r="E486" s="9">
         <f t="shared" si="86"/>
-        <v>5400</v>
+        <v>64800</v>
       </c>
       <c r="H486" s="4">
         <v>70000</v>
       </c>
       <c r="I486" s="4">
         <f>E486</f>
-        <v>5400</v>
+        <v>64800</v>
       </c>
       <c r="J486" s="4" t="s">
         <v>229</v>
@@ -16056,14 +16056,14 @@
       </c>
       <c r="E487" s="9">
         <f t="shared" si="86"/>
-        <v>4800</v>
+        <v>57600</v>
       </c>
       <c r="H487" s="4">
         <v>62400</v>
       </c>
       <c r="I487" s="4">
         <f>E487</f>
-        <v>4800</v>
+        <v>57600</v>
       </c>
       <c r="K487" s="9">
         <v>4800</v>
@@ -16084,7 +16084,7 @@
       </c>
       <c r="E488" s="9">
         <f t="shared" si="86"/>
-        <v>8200</v>
+        <v>98400</v>
       </c>
       <c r="F488" s="4">
         <v>26000</v>
@@ -16143,8 +16143,8 @@
         <v>6</v>
       </c>
       <c r="E490" s="9">
-        <f t="shared" ref="E490:E498" si="87">K490</f>
-        <v>8200</v>
+        <f t="shared" ref="E490:E498" si="87">K490*12</f>
+        <v>98400</v>
       </c>
       <c r="F490" s="4">
         <v>26000</v>
@@ -16157,7 +16157,7 @@
       </c>
       <c r="I490" s="4">
         <f t="shared" ref="I490:I492" si="88">E490*3</f>
-        <v>24600</v>
+        <v>295200</v>
       </c>
       <c r="J490" s="4" t="s">
         <v>86</v>
@@ -16181,7 +16181,7 @@
       </c>
       <c r="E491" s="9">
         <f t="shared" si="87"/>
-        <v>8000</v>
+        <v>96000</v>
       </c>
       <c r="F491" s="4">
         <v>20000</v>
@@ -16191,7 +16191,7 @@
       </c>
       <c r="I491" s="4">
         <f t="shared" si="88"/>
-        <v>24000</v>
+        <v>288000</v>
       </c>
       <c r="K491" s="4">
         <v>8000</v>
@@ -16212,7 +16212,7 @@
       </c>
       <c r="E492" s="9">
         <f t="shared" si="87"/>
-        <v>7900</v>
+        <v>94800</v>
       </c>
       <c r="F492" s="4">
         <v>0</v>
@@ -16225,7 +16225,7 @@
       </c>
       <c r="I492" s="4">
         <f t="shared" si="88"/>
-        <v>23700</v>
+        <v>284400</v>
       </c>
       <c r="K492" s="4">
         <v>7900</v>
@@ -16246,7 +16246,7 @@
       </c>
       <c r="E493" s="9">
         <f t="shared" si="87"/>
-        <v>7900</v>
+        <v>94800</v>
       </c>
       <c r="F493" s="4">
         <v>22000</v>
@@ -16260,7 +16260,7 @@
       </c>
       <c r="I493" s="4">
         <f>E493*3</f>
-        <v>23700</v>
+        <v>284400</v>
       </c>
       <c r="J493" s="4" t="s">
         <v>94</v>
@@ -16284,7 +16284,7 @@
       </c>
       <c r="E494" s="9">
         <f t="shared" si="87"/>
-        <v>7500</v>
+        <v>90000</v>
       </c>
       <c r="F494" s="4">
         <v>10000</v>
@@ -16298,7 +16298,7 @@
       </c>
       <c r="I494" s="4">
         <f>E494*1.5</f>
-        <v>11250</v>
+        <v>135000</v>
       </c>
       <c r="K494" s="4">
         <v>7500</v>
@@ -16319,7 +16319,7 @@
       </c>
       <c r="E495" s="9">
         <f t="shared" si="87"/>
-        <v>7500</v>
+        <v>90000</v>
       </c>
       <c r="F495" s="4">
         <v>0</v>
@@ -16332,7 +16332,7 @@
       </c>
       <c r="I495" s="4">
         <f>E495*3</f>
-        <v>22500</v>
+        <v>270000</v>
       </c>
       <c r="J495" s="4" t="s">
         <v>104</v>
@@ -16356,7 +16356,7 @@
       </c>
       <c r="E496" s="9">
         <f t="shared" si="87"/>
-        <v>7400</v>
+        <v>88800</v>
       </c>
       <c r="F496" s="4">
         <v>25000</v>
@@ -16366,7 +16366,7 @@
       </c>
       <c r="I496" s="4">
         <f>E496*1.5</f>
-        <v>11100</v>
+        <v>133200</v>
       </c>
       <c r="K496" s="9">
         <v>7400</v>
@@ -16387,14 +16387,14 @@
       </c>
       <c r="E497" s="9">
         <f t="shared" si="87"/>
-        <v>7200</v>
+        <v>86400</v>
       </c>
       <c r="H497" s="4">
         <v>86400</v>
       </c>
       <c r="I497" s="4">
         <f>E497*3</f>
-        <v>21600</v>
+        <v>259200</v>
       </c>
       <c r="K497" s="4">
         <v>7200</v>
@@ -16415,14 +16415,14 @@
       </c>
       <c r="E498" s="9">
         <f t="shared" si="87"/>
-        <v>7000</v>
+        <v>84000</v>
       </c>
       <c r="H498" s="4">
         <v>94500</v>
       </c>
       <c r="I498" s="4">
         <f>E498*1.5</f>
-        <v>10500</v>
+        <v>126000</v>
       </c>
       <c r="J498" s="4" t="s">
         <v>121</v>
@@ -16619,8 +16619,8 @@
         <v>6</v>
       </c>
       <c r="E506" s="9">
-        <f>K506</f>
-        <v>3200</v>
+        <f>K506*12</f>
+        <v>38400</v>
       </c>
       <c r="G506" s="4">
         <v>500</v>
@@ -16671,8 +16671,8 @@
         <v>6</v>
       </c>
       <c r="E508" s="9">
-        <f t="shared" ref="E508:E511" si="90">K508</f>
-        <v>7200</v>
+        <f t="shared" ref="E508:E511" si="90">K508*12</f>
+        <v>86400</v>
       </c>
       <c r="F508" s="4">
         <v>0</v>
@@ -16685,7 +16685,7 @@
       </c>
       <c r="I508" s="4">
         <f>E508*3</f>
-        <v>21600</v>
+        <v>259200</v>
       </c>
       <c r="J508" s="4" t="s">
         <v>108</v>
@@ -16709,7 +16709,7 @@
       </c>
       <c r="E509" s="9">
         <f t="shared" si="90"/>
-        <v>7400</v>
+        <v>88800</v>
       </c>
       <c r="F509" s="4">
         <v>20000</v>
@@ -16722,7 +16722,7 @@
       </c>
       <c r="I509" s="4">
         <f>E509*1.5</f>
-        <v>11100</v>
+        <v>133200</v>
       </c>
       <c r="J509" s="4" t="s">
         <v>105</v>
@@ -16746,14 +16746,14 @@
       </c>
       <c r="E510" s="9">
         <f t="shared" si="90"/>
-        <v>6000</v>
+        <v>72000</v>
       </c>
       <c r="H510" s="4">
         <v>95000</v>
       </c>
       <c r="I510" s="4">
         <f>E510</f>
-        <v>6000</v>
+        <v>72000</v>
       </c>
       <c r="J510" s="4" t="s">
         <v>172</v>
@@ -16777,7 +16777,7 @@
       </c>
       <c r="E511" s="9">
         <f t="shared" si="90"/>
-        <v>4913</v>
+        <v>58956</v>
       </c>
       <c r="F511" s="4">
         <v>0</v>
@@ -16917,8 +16917,8 @@
         <v>199</v>
       </c>
       <c r="E516" s="9">
-        <f t="shared" ref="E516:E523" si="92">K516</f>
-        <v>5600</v>
+        <f t="shared" ref="E516:E523" si="92">K516*12</f>
+        <v>67200</v>
       </c>
       <c r="H516">
         <f>K516*12</f>
@@ -16949,7 +16949,7 @@
       </c>
       <c r="E517" s="9">
         <f t="shared" si="92"/>
-        <v>5400</v>
+        <v>64800</v>
       </c>
       <c r="H517">
         <f>K517*12</f>
@@ -16980,7 +16980,7 @@
       </c>
       <c r="E518" s="9">
         <f t="shared" si="92"/>
-        <v>5000</v>
+        <v>60000</v>
       </c>
       <c r="H518">
         <f>K518*12</f>
@@ -17011,7 +17011,7 @@
       </c>
       <c r="E519" s="9">
         <f t="shared" si="92"/>
-        <v>5000</v>
+        <v>60000</v>
       </c>
       <c r="H519">
         <f>K519*12</f>
@@ -17042,7 +17042,7 @@
       </c>
       <c r="E520" s="9">
         <f t="shared" si="92"/>
-        <v>5000</v>
+        <v>60000</v>
       </c>
       <c r="H520">
         <f>K520*12</f>
@@ -17073,7 +17073,7 @@
       </c>
       <c r="E521" s="9">
         <f t="shared" si="92"/>
-        <v>3800</v>
+        <v>45600</v>
       </c>
       <c r="F521" s="4">
         <v>0</v>
@@ -17109,7 +17109,7 @@
       </c>
       <c r="E522" s="9">
         <f t="shared" si="92"/>
-        <v>3700</v>
+        <v>44400</v>
       </c>
       <c r="H522">
         <f>K522*12</f>
@@ -17137,7 +17137,7 @@
       </c>
       <c r="E523" s="9">
         <f t="shared" si="92"/>
-        <v>3600</v>
+        <v>43200</v>
       </c>
       <c r="F523" s="4">
         <v>0</v>
@@ -17284,8 +17284,8 @@
         <v>6</v>
       </c>
       <c r="E528" s="9">
-        <f t="shared" ref="E528:E529" si="94">K528</f>
-        <v>5600</v>
+        <f t="shared" ref="E528:E529" si="94">K528*12</f>
+        <v>67200</v>
       </c>
       <c r="F528" s="4" t="s">
         <v>18</v>
@@ -17319,7 +17319,7 @@
       </c>
       <c r="E529" s="9">
         <f t="shared" si="94"/>
-        <v>5000</v>
+        <v>60000</v>
       </c>
       <c r="H529">
         <f>K529*12</f>
@@ -17382,8 +17382,8 @@
         <v>6</v>
       </c>
       <c r="E531" s="9">
-        <f t="shared" ref="E531:E535" si="95">K531</f>
-        <v>7000</v>
+        <f t="shared" ref="E531:E535" si="95">K531*12</f>
+        <v>84000</v>
       </c>
       <c r="G531" s="4">
         <v>10000</v>
@@ -17413,7 +17413,7 @@
       </c>
       <c r="E532" s="9">
         <f t="shared" si="95"/>
-        <v>6200</v>
+        <v>74400</v>
       </c>
       <c r="F532" s="4">
         <v>10000</v>
@@ -17448,7 +17448,7 @@
       </c>
       <c r="E533" s="9">
         <f t="shared" si="95"/>
-        <v>6000</v>
+        <v>72000</v>
       </c>
       <c r="F533" s="4">
         <v>10000</v>
@@ -17485,7 +17485,7 @@
       </c>
       <c r="E534" s="9">
         <f t="shared" si="95"/>
-        <v>6000</v>
+        <v>72000</v>
       </c>
       <c r="F534" s="4">
         <v>10000</v>
@@ -17523,7 +17523,7 @@
       </c>
       <c r="E535" s="9">
         <f t="shared" si="95"/>
-        <v>6000</v>
+        <v>72000</v>
       </c>
       <c r="F535" s="4">
         <v>10000</v>
@@ -17826,8 +17826,8 @@
         <v>6</v>
       </c>
       <c r="E547" s="9">
-        <f t="shared" ref="E547:E548" si="98">K547</f>
-        <v>11666.666666666666</v>
+        <f t="shared" ref="E547:E548" si="98">K547*12</f>
+        <v>140000</v>
       </c>
       <c r="H547" s="4">
         <v>160000</v>
@@ -17855,7 +17855,7 @@
       </c>
       <c r="E548" s="9">
         <f t="shared" si="98"/>
-        <v>11666.666666666666</v>
+        <v>140000</v>
       </c>
       <c r="F548" s="4">
         <v>20000</v>
@@ -18017,8 +18017,8 @@
         <v>6</v>
       </c>
       <c r="E554" s="9">
-        <f t="shared" ref="E554:E556" si="100">K554</f>
-        <v>8333.3333333333339</v>
+        <f t="shared" ref="E554:E556" si="100">K554*12</f>
+        <v>100000</v>
       </c>
       <c r="F554" s="4">
         <v>55000</v>
@@ -18052,7 +18052,7 @@
       </c>
       <c r="E555" s="9">
         <f t="shared" si="100"/>
-        <v>8200</v>
+        <v>98400</v>
       </c>
       <c r="F555" s="4">
         <v>50000</v>
@@ -18086,7 +18086,7 @@
       </c>
       <c r="E556" s="9">
         <f t="shared" si="100"/>
-        <v>7000</v>
+        <v>84000</v>
       </c>
       <c r="H556">
         <f>K556*12</f>

</xml_diff>